<commit_message>
rerun survival analysis with K28-altered cohort
</commit_message>
<xml_diff>
--- a/analyses/08-survival/output/Table-S4.xlsx
+++ b/analyses/08-survival/output/Table-S4.xlsx
@@ -52,133 +52,133 @@
     <t xml:space="preserve">BS_79NQJZ09</t>
   </si>
   <si>
+    <t xml:space="preserve">BS_9DM8H1RX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_ABZ3BK38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_D6XHKZDZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_E42SSQGJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_F064HMTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_F8K4VQMF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_KSHETTQC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_KXGJ1HMG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_M4E4H6NG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_M5FM63EB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_MSB1RDAJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_MW63FCZC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_NJFK43N3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_P3PF53V8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_QWS88QXE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_R1G6SG0K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_S791VC80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_SK4H5MJQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_SKRY0BJ4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_W2QCHQ7E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_WJB33V17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_XGVSX8BX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_20TBZG09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H3 WT, ALT +</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_3NX3RBCX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_79SYEHY3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_80078QDG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_EJV0N3BX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_EP25TTAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_G9MQM1KK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_HJ95JNFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_JB3J82ZK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_RG6JK7ZN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_S0T3CQ97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_VW4XN9Y7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_1S5V7WWC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H3 K28, ALT -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_3E5C1PN1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_3Z40EZHD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_7GKF6M85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_823V5X6Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BS_872Q3FK2</t>
+  </si>
+  <si>
     <t xml:space="preserve">BS_8FSJDG2T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_9DM8H1RX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_ABZ3BK38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_D6XHKZDZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_E42SSQGJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_F064HMTP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_F8K4VQMF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_KSHETTQC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_KXGJ1HMG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_M4E4H6NG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_M5FM63EB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_MSB1RDAJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_MW63FCZC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_NJFK43N3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_P3PF53V8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_QWS88QXE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_R1G6SG0K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_S791VC80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_SK4H5MJQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_SKRY0BJ4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_W2QCHQ7E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_WJB33V17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_XGVSX8BX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_20TBZG09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H3 WT, ALT +</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_3NX3RBCX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_79SYEHY3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_80078QDG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_EJV0N3BX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_EP25TTAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_G9MQM1KK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_HJ95JNFN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_JB3J82ZK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_RG6JK7ZN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_S0T3CQ97</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_VW4XN9Y7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_1S5V7WWC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H3 K28, ALT -</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_3E5C1PN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_3Z40EZHD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_7GKF6M85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_823V5X6Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BS_872Q3FK2</t>
   </si>
   <si>
     <t xml:space="preserve">BS_AFAHY6HP</t>
@@ -769,7 +769,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="n">
-        <v>12.7889009435513</v>
+        <v>0.328763520399776</v>
       </c>
     </row>
     <row r="9">
@@ -783,7 +783,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="n">
-        <v>0.328763520399776</v>
+        <v>39.0899825755334</v>
       </c>
     </row>
     <row r="10">
@@ -797,7 +797,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>39.0899825755334</v>
+        <v>233.783739356281</v>
       </c>
     </row>
     <row r="11">
@@ -811,7 +811,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="n">
-        <v>233.783739356281</v>
+        <v>16.9313213005885</v>
       </c>
     </row>
     <row r="12">
@@ -824,8 +824,8 @@
       <c r="C12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" t="n">
-        <v>16.9313213005885</v>
+      <c r="D12" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="13">
@@ -838,8 +838,8 @@
       <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="D13" t="e">
-        <v>#N/A</v>
+      <c r="D13" t="n">
+        <v>16.175165203669</v>
       </c>
     </row>
     <row r="14">
@@ -853,7 +853,7 @@
         <v>6</v>
       </c>
       <c r="D14" t="n">
-        <v>16.175165203669</v>
+        <v>58.3884012230003</v>
       </c>
     </row>
     <row r="15">
@@ -867,7 +867,7 @@
         <v>6</v>
       </c>
       <c r="D15" t="n">
-        <v>58.3884012230003</v>
+        <v>28.1092809941809</v>
       </c>
     </row>
     <row r="16">
@@ -881,7 +881,7 @@
         <v>6</v>
       </c>
       <c r="D16" t="n">
-        <v>28.1092809941809</v>
+        <v>49.5775388762863</v>
       </c>
     </row>
     <row r="17">
@@ -895,7 +895,7 @@
         <v>6</v>
       </c>
       <c r="D17" t="n">
-        <v>49.5775388762863</v>
+        <v>12.9861590557912</v>
       </c>
     </row>
     <row r="18">
@@ -909,7 +909,7 @@
         <v>6</v>
       </c>
       <c r="D18" t="n">
-        <v>12.9861590557912</v>
+        <v>12.3286320149916</v>
       </c>
     </row>
     <row r="19">
@@ -923,7 +923,7 @@
         <v>6</v>
       </c>
       <c r="D19" t="n">
-        <v>12.3286320149916</v>
+        <v>86.2675477529013</v>
       </c>
     </row>
     <row r="20">
@@ -936,8 +936,8 @@
       <c r="C20" t="s">
         <v>6</v>
       </c>
-      <c r="D20" t="n">
-        <v>86.2675477529013</v>
+      <c r="D20" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="21">
@@ -950,8 +950,8 @@
       <c r="C21" t="s">
         <v>6</v>
       </c>
-      <c r="D21" t="e">
-        <v>#N/A</v>
+      <c r="D21" t="n">
+        <v>40.0762731367327</v>
       </c>
     </row>
     <row r="22">
@@ -965,7 +965,7 @@
         <v>6</v>
       </c>
       <c r="D22" t="n">
-        <v>40.0762731367327</v>
+        <v>21.3038761219055</v>
       </c>
     </row>
     <row r="23">
@@ -979,7 +979,7 @@
         <v>6</v>
       </c>
       <c r="D23" t="n">
-        <v>21.3038761219055</v>
+        <v>11.0793306374725</v>
       </c>
     </row>
     <row r="24">
@@ -993,7 +993,7 @@
         <v>6</v>
       </c>
       <c r="D24" t="n">
-        <v>11.0793306374725</v>
+        <v>31.4626689022586</v>
       </c>
     </row>
     <row r="25">
@@ -1007,7 +1007,7 @@
         <v>6</v>
       </c>
       <c r="D25" t="n">
-        <v>31.4626689022586</v>
+        <v>11.835486734392</v>
       </c>
     </row>
     <row r="26">
@@ -1021,7 +1021,7 @@
         <v>6</v>
       </c>
       <c r="D26" t="n">
-        <v>11.835486734392</v>
+        <v>16.9313213005885</v>
       </c>
     </row>
     <row r="27">
@@ -1035,7 +1035,7 @@
         <v>6</v>
       </c>
       <c r="D27" t="n">
-        <v>16.9313213005885</v>
+        <v>84.1963375743827</v>
       </c>
     </row>
     <row r="28">
@@ -1049,7 +1049,7 @@
         <v>6</v>
       </c>
       <c r="D28" t="n">
-        <v>84.1963375743827</v>
+        <v>54.5747443863629</v>
       </c>
     </row>
     <row r="29">
@@ -1063,7 +1063,7 @@
         <v>6</v>
       </c>
       <c r="D29" t="n">
-        <v>54.5747443863629</v>
+        <v>7.29855015287504</v>
       </c>
     </row>
     <row r="30">
@@ -1074,24 +1074,24 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D30" t="n">
-        <v>7.29855015287504</v>
+        <v>17.9833645658678</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
         <v>35</v>
       </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>36</v>
-      </c>
       <c r="D31" t="n">
-        <v>17.9833645658678</v>
+        <v>272.249071243055</v>
       </c>
     </row>
     <row r="32">
@@ -1102,10 +1102,10 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" t="n">
-        <v>272.249071243055</v>
+        <v>108.327579971726</v>
       </c>
     </row>
     <row r="33">
@@ -1116,10 +1116,10 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D33" t="n">
-        <v>108.327579971726</v>
+        <v>11.4738468619522</v>
       </c>
     </row>
     <row r="34">
@@ -1130,10 +1130,10 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D34" t="n">
-        <v>11.4738468619522</v>
+        <v>13.8738205608706</v>
       </c>
     </row>
     <row r="35">
@@ -1144,10 +1144,10 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D35" t="n">
-        <v>13.8738205608706</v>
+        <v>17.1285794128284</v>
       </c>
     </row>
     <row r="36">
@@ -1158,10 +1158,10 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D36" t="n">
-        <v>17.1285794128284</v>
+        <v>167.669395403886</v>
       </c>
     </row>
     <row r="37">
@@ -1172,10 +1172,10 @@
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" t="n">
-        <v>167.669395403886</v>
+        <v>52.4706578558043</v>
       </c>
     </row>
     <row r="38">
@@ -1186,10 +1186,10 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38" t="n">
-        <v>52.4706578558043</v>
+        <v>2.46572640299832</v>
       </c>
     </row>
     <row r="39">
@@ -1200,10 +1200,10 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D39" t="n">
-        <v>2.46572640299832</v>
+        <v>44.3173225498899</v>
       </c>
     </row>
     <row r="40">
@@ -1214,10 +1214,10 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D40" t="n">
-        <v>44.3173225498899</v>
+        <v>37.4461649735345</v>
       </c>
     </row>
     <row r="41">
@@ -1228,10 +1228,10 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D41" t="n">
-        <v>37.4461649735345</v>
+        <v>10.9807015813525</v>
       </c>
     </row>
     <row r="42">
@@ -1242,24 +1242,24 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D42" t="n">
-        <v>10.9807015813525</v>
+        <v>26.7613505605418</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D43" t="n">
-        <v>26.7613505605418</v>
+        <v>13.7751915047506</v>
       </c>
     </row>
     <row r="44">
@@ -1270,10 +1270,10 @@
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D44" t="n">
-        <v>13.7751915047506</v>
+        <v>5.62185619883618</v>
       </c>
     </row>
     <row r="45">
@@ -1284,10 +1284,10 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D45" t="n">
-        <v>5.62185619883618</v>
+        <v>12.9532827037512</v>
       </c>
     </row>
     <row r="46">
@@ -1298,10 +1298,10 @@
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D46" t="n">
-        <v>12.9532827037512</v>
+        <v>9.66564749975343</v>
       </c>
     </row>
     <row r="47">
@@ -1312,10 +1312,10 @@
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D47" t="n">
-        <v>9.66564749975343</v>
+        <v>23.2107045402242</v>
       </c>
     </row>
     <row r="48">
@@ -1326,10 +1326,10 @@
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D48" t="n">
-        <v>23.2107045402242</v>
+        <v>12.7889009435513</v>
       </c>
     </row>
     <row r="49">
@@ -1340,7 +1340,7 @@
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D49" t="n">
         <v>3.28763520399776</v>
@@ -1354,7 +1354,7 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50" t="n">
         <v>9.07387316303383</v>
@@ -1368,7 +1368,7 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D51" t="n">
         <v>2.00545747443864</v>
@@ -1382,7 +1382,7 @@
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D52" t="n">
         <v>9.00812045895387</v>
@@ -1396,7 +1396,7 @@
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D53" t="n">
         <v>0.394516224479732</v>
@@ -1410,7 +1410,7 @@
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D54" t="n">
         <v>28.9969424992603</v>
@@ -1424,7 +1424,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D55" t="n">
         <v>5.884867015156</v>
@@ -1438,7 +1438,7 @@
         <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D56" t="n">
         <v>8.02182989775454</v>
@@ -1452,7 +1452,7 @@
         <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D57" t="n">
         <v>11.769734030312</v>
@@ -1466,7 +1466,7 @@
         <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D58" t="n">
         <v>17.2272084689483</v>
@@ -1480,7 +1480,7 @@
         <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D59" t="n">
         <v>1.28217772955913</v>
@@ -1494,7 +1494,7 @@
         <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D60" t="n">
         <v>18.1477463260677</v>
@@ -1508,7 +1508,7 @@
         <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D61" t="n">
         <v>51.5829963507249</v>
@@ -1522,7 +1522,7 @@
         <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D62" t="n">
         <v>17.621724693428</v>
@@ -1536,7 +1536,7 @@
         <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D63" t="n">
         <v>0.591774336719598</v>
@@ -1550,7 +1550,7 @@
         <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D64" t="n">
         <v>7.39717920899497</v>
@@ -1564,7 +1564,7 @@
         <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D65" t="n">
         <v>8.9752441069139</v>
@@ -1578,7 +1578,7 @@
         <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D66" t="n">
         <v>7.92320084163461</v>
@@ -1894,15 +1894,15 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>28.1092809941809</v>
+        <v>29.7859749482197</v>
       </c>
       <c r="C2" t="n">
-        <v>59.7399686225618</v>
+        <v>60.4584263587911</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="n">
         <v>27.7147647697012</v>
@@ -1913,13 +1913,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="n">
-        <v>9.04099681099385</v>
+        <v>9.07387316303383</v>
       </c>
       <c r="C4" t="n">
-        <v>11.444015723099</v>
+        <v>11.2031646824284</v>
       </c>
     </row>
     <row r="5">
@@ -1980,16 +1980,16 @@
         <v>102</v>
       </c>
       <c r="B2" t="n">
-        <v>1.23800683567383</v>
+        <v>1.26744316288693</v>
       </c>
       <c r="C2" t="n">
-        <v>0.638878704958487</v>
+        <v>0.639748511347808</v>
       </c>
       <c r="D2" t="n">
-        <v>1.93778071810091</v>
+        <v>1.98115844023883</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0526499811778664</v>
+        <v>0.0475735082591508</v>
       </c>
     </row>
     <row r="3">
@@ -1997,16 +1997,16 @@
         <v>103</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.128950610885961</v>
+        <v>-0.148237286588846</v>
       </c>
       <c r="C3" t="n">
-        <v>0.641264221730018</v>
+        <v>0.642047340575248</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.201088110822829</v>
+        <v>-0.230882175224075</v>
       </c>
       <c r="E3" t="n">
-        <v>0.840629678305721</v>
+        <v>0.817406338760701</v>
       </c>
     </row>
     <row r="4">
@@ -2014,16 +2014,16 @@
         <v>104</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.250511175106721</v>
+        <v>-0.238394081195341</v>
       </c>
       <c r="C4" t="n">
-        <v>0.261684444016358</v>
+        <v>0.261419868381904</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.957302510083715</v>
+        <v>-0.911920286208222</v>
       </c>
       <c r="E4" t="n">
-        <v>0.338414588782397</v>
+        <v>0.361810681706881</v>
       </c>
     </row>
   </sheetData>

</xml_diff>